<commit_message>
change result file to match test zip file
</commit_message>
<xml_diff>
--- a/test/Invoices.xlsx
+++ b/test/Invoices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Invoice Number</t>
   </si>
@@ -28,10 +28,16 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>2016.12.01</t>
-  </si>
-  <si>
-    <t>2017.02.03</t>
+    <t>2016.11.07</t>
+  </si>
+  <si>
+    <t>2017.01.11</t>
+  </si>
+  <si>
+    <t>2017.01.09</t>
+  </si>
+  <si>
+    <t>2016.11.08</t>
   </si>
 </sst>
 </file>
@@ -363,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E16"/>
+  <dimension ref="B1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,7 +391,7 @@
     </row>
     <row r="2" spans="2:5">
       <c r="B2">
-        <v>6511652116</v>
+        <v>6510848763</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -394,82 +400,82 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>1125685</v>
+        <v>266915</v>
       </c>
     </row>
     <row r="3" spans="2:5">
       <c r="B3">
-        <v>6511652118</v>
+        <v>6510848803</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>16330</v>
+        <v>245895</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4">
-        <v>6511652120</v>
+        <v>6510848932</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>5446290</v>
+        <v>1018340</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="B5">
-        <v>6511652123</v>
+        <v>6510849001</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5">
-        <v>190860</v>
+        <v>964590</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6">
-        <v>6511652128</v>
+        <v>6510849079</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6">
-        <v>131535</v>
+        <v>248455</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7">
-        <v>6511652131</v>
+        <v>6510849149</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>718770</v>
+        <v>1074500</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8">
-        <v>6511652134</v>
+        <v>6510849460</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -478,119 +484,21 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <v>2947735</v>
+        <v>36895</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9">
-        <v>6511652138</v>
+        <v>6510849534</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9">
-        <v>2121345</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10">
-        <v>6511652140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>365375</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11">
-        <v>6511652145</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>365375</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12">
-        <v>6511652147</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>591125</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13">
-        <v>6511652150</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>718770</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14">
-        <v>6511652152</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>272975</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15">
-        <v>6511652155</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <v>19770</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16">
-        <v>6511652179</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>22495</v>
+        <v>26085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>